<commit_message>
update new task for task2
</commit_message>
<xml_diff>
--- a/isitword test/ref/dict.xlsx
+++ b/isitword test/ref/dict.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E81"/>
+  <dimension ref="A1:F81"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -459,465 +459,542 @@
           <t>len</t>
         </is>
       </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>actual len</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>รถบัส</t>
+          <t>แมว</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>รัถสบ</t>
+          <t>มวแ</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>รพท้น</t>
+          <t>แรน</t>
         </is>
       </c>
       <c r="E2" t="n">
-        <v>5</v>
+        <v>3</v>
+      </c>
+      <c r="F2" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>3</v>
+        <v>27</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>แมว</t>
+          <t>หวี</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>มวแ</t>
+          <t>วหี</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>แรน</t>
+          <t>หวึ</t>
         </is>
       </c>
       <c r="E3" t="n">
         <v>3</v>
+      </c>
+      <c r="F3" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>6</v>
+        <v>42</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>ปากกา</t>
+          <t>อิฐ</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>าากปก</t>
+          <t>ฐอิ</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>ปลบกน</t>
+          <t>อิฎ</t>
         </is>
       </c>
       <c r="E4" t="n">
-        <v>5</v>
+        <v>3</v>
+      </c>
+      <c r="F4" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>7</v>
+        <v>64</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>หมวก</t>
+          <t>สมอ</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>หวมก</t>
+          <t>มสอ</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>หนนา</t>
+          <t>สวก</t>
         </is>
       </c>
       <c r="E5" t="n">
-        <v>4</v>
+        <v>3</v>
+      </c>
+      <c r="F5" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="n">
-        <v>8</v>
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>c1</t>
+        </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>เลื่อย</t>
+          <t>กาว</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>ล่เอืย</t>
+          <t>วกา</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>เกี๊ยน</t>
+          <t>ถาว</t>
         </is>
       </c>
       <c r="E6" t="n">
-        <v>6</v>
+        <v>3</v>
+      </c>
+      <c r="F6" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="n">
-        <v>9</v>
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>c2</t>
+        </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>คันธนู</t>
+          <t>ผัก</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>นคูนัธ</t>
+          <t>กผั</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>คัรหบุ</t>
+          <t>พัภ</t>
         </is>
       </c>
       <c r="E7" t="n">
-        <v>6</v>
+        <v>3</v>
+      </c>
+      <c r="F7" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="n">
-        <v>10</v>
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>c3</t>
+        </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>ค้างคาว</t>
+          <t>ดิน</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>คาค้วาง</t>
+          <t>ดนิ</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>ค้นถาพล</t>
+          <t>มิท</t>
         </is>
       </c>
       <c r="E8" t="n">
-        <v>7</v>
+        <v>3</v>
+      </c>
+      <c r="F8" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="n">
-        <v>11</v>
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>c4</t>
+        </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>เหยือก</t>
+          <t>หมา</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>กหืยอเ</t>
+          <t>มาห</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>เกนีทน</t>
+          <t>ทนา</t>
         </is>
       </c>
       <c r="E9" t="n">
-        <v>6</v>
+        <v>3</v>
+      </c>
+      <c r="F9" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>หนังสือ</t>
+          <t>หมวก</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>สัหอืนง</t>
+          <t>หวมก</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>หกันพีบ</t>
+          <t>หนนา</t>
         </is>
       </c>
       <c r="E10" t="n">
-        <v>7</v>
+        <v>4</v>
+      </c>
+      <c r="F10" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>ลูกแพร์</t>
+          <t>เรือ</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>พูก์แรล</t>
+          <t>อืเร</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>ลูนธาน์</t>
+          <t>เติน</t>
         </is>
       </c>
       <c r="E11" t="n">
-        <v>7</v>
+        <v>4</v>
+      </c>
+      <c r="F11" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>24</v>
+        <v>51</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>ไม้เท้า</t>
+          <t>โซฟา</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>ท้เาไม้</t>
+          <t>โฟซา</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>ไย้นทีล</t>
+          <t>โผฝบ</t>
         </is>
       </c>
       <c r="E12" t="n">
-        <v>7</v>
+        <v>4</v>
+      </c>
+      <c r="F12" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>26</v>
+        <v>63</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>แจกัน</t>
+          <t>หมอน</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>กนแจั</t>
+          <t>นอมห</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>แสนืร</t>
+          <t>หนตบ</t>
         </is>
       </c>
       <c r="E13" t="n">
-        <v>5</v>
+        <v>4</v>
+      </c>
+      <c r="F13" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>27</v>
+        <v>68</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>หวี</t>
+          <t>กุ้ง</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>วหี</t>
+          <t>กงุ้</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>หวึ</t>
+          <t>กู่บ</t>
         </is>
       </c>
       <c r="E14" t="n">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="F14" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" t="n">
-        <v>28</v>
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>75a</t>
+        </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>ของขวัญ</t>
+          <t>มะยม</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>ขัวองญข</t>
+          <t>มยะม</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>ขนาผฟีล</t>
+          <t>นะบม</t>
         </is>
       </c>
       <c r="E15" t="n">
-        <v>7</v>
+        <v>4</v>
+      </c>
+      <c r="F15" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>30</v>
+        <v>93</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>เรือ</t>
+          <t>โลมา</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>อืเร</t>
+          <t>มโลา</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>เติน</t>
+          <t>โบลม</t>
         </is>
       </c>
       <c r="E16" t="n">
         <v>4</v>
       </c>
+      <c r="F16" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="17">
-      <c r="A17" t="n">
-        <v>31</v>
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>d1</t>
+        </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>เข็มขัด</t>
+          <t>กวาง</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>ขเดมัข็</t>
+          <t>วงาก</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>เน้บลีต</t>
+          <t>ถาวง</t>
         </is>
       </c>
       <c r="E17" t="n">
-        <v>7</v>
+        <v>4</v>
+      </c>
+      <c r="F17" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>41</v>
+        <v>6</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>สว่าน</t>
+          <t>ปากกา</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>นวาส่</t>
+          <t>าากปก</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>สยึนบ</t>
+          <t>ปลบกน</t>
         </is>
       </c>
       <c r="E18" t="n">
+        <v>5</v>
+      </c>
+      <c r="F18" t="n">
         <v>5</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>42</v>
+        <v>26</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>อิฐ</t>
+          <t>แจกัน</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>ฐอิ</t>
+          <t>กนแจั</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>อิฎ</t>
+          <t>แสนืร</t>
         </is>
       </c>
       <c r="E19" t="n">
-        <v>3</v>
+        <v>5</v>
+      </c>
+      <c r="F19" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>ลูกอม</t>
+          <t>สว่าน</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>กมลอู</t>
+          <t>นวาส่</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>ลุนทา</t>
+          <t>สยึนบ</t>
         </is>
       </c>
       <c r="E20" t="n">
         <v>5</v>
+      </c>
+      <c r="F20" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>โดนัท</t>
+          <t>ลูกอม</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>ดทนัโ</t>
+          <t>กมลอู</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>โตคีก</t>
+          <t>ลุนทา</t>
         </is>
       </c>
       <c r="E21" t="n">
         <v>5</v>
+      </c>
+      <c r="F21" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="22">
@@ -942,442 +1019,506 @@
       <c r="E22" t="n">
         <v>5</v>
       </c>
+      <c r="F22" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>ดอกไม้</t>
+          <t>องุ่น</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>ดก้ไอม</t>
+          <t>นุง่อ</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>ดวลโข้</t>
+          <t>อตู๊บ</t>
         </is>
       </c>
       <c r="E23" t="n">
-        <v>6</v>
+        <v>5</v>
+      </c>
+      <c r="F23" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>51</v>
+        <v>66</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>โซฟา</t>
+          <t>ยางลบ</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>โฟซา</t>
+          <t>บายงล</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>โผฝบ</t>
+          <t>ยอนวบ</t>
         </is>
       </c>
       <c r="E24" t="n">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="F24" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>52</v>
+        <v>87</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>องุ่น</t>
+          <t>นกยูง</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>นุง่อ</t>
+          <t>ยูกนง</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>อตู๊บ</t>
+          <t>นดถูค</t>
         </is>
       </c>
       <c r="E25" t="n">
         <v>5</v>
+      </c>
+      <c r="F25" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>61</v>
+        <v>8</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>รูปปั้น</t>
+          <t>เลื่อย</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>ป้ปันรู</t>
+          <t>ล่เอืย</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>รูฟฝื้อ</t>
+          <t>เกี๊ยน</t>
         </is>
       </c>
       <c r="E26" t="n">
-        <v>7</v>
+        <v>6</v>
+      </c>
+      <c r="F26" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>63</v>
+        <v>11</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>หมอน</t>
+          <t>เหยือก</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>นอมห</t>
+          <t>กหืยอเ</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>หนตบ</t>
+          <t>เกนีทน</t>
         </is>
       </c>
       <c r="E27" t="n">
-        <v>4</v>
+        <v>6</v>
+      </c>
+      <c r="F27" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>64</v>
+        <v>50</v>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>สมอ</t>
+          <t>ดอกไม้</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>มสอ</t>
+          <t>ดก้ไอม</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>สวก</t>
+          <t>ดวลโข้</t>
         </is>
       </c>
       <c r="E28" t="n">
-        <v>3</v>
+        <v>6</v>
+      </c>
+      <c r="F28" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>ยางลบ</t>
+          <t>ฟองน้ำ</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>บายงล</t>
+          <t>อำนฟ้ง</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>ยอนวบ</t>
+          <t>ฟวยวิ้บ</t>
         </is>
       </c>
       <c r="E29" t="n">
+        <v>6</v>
+      </c>
+      <c r="F29" t="n">
         <v>5</v>
       </c>
     </row>
     <row r="30">
-      <c r="A30" t="n">
-        <v>68</v>
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>71a</t>
+        </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>กุ้ง</t>
+          <t>ตะหลิว</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>กงุ้</t>
+          <t>วิหะตล</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>กู่บ</t>
+          <t>ดะหลิว</t>
         </is>
       </c>
       <c r="E30" t="n">
-        <v>4</v>
+        <v>6</v>
+      </c>
+      <c r="F30" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>70</v>
+        <v>82</v>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>ฟองน้ำ</t>
+          <t>แว่นตา</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>อำนฟ้ง</t>
+          <t>ว่าตนแ</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>ฟวยวิ้บ</t>
+          <t>แย้บคา</t>
         </is>
       </c>
       <c r="E31" t="n">
         <v>6</v>
       </c>
+      <c r="F31" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>71</v>
+        <v>88</v>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>คุกกี้</t>
+          <t>น้ำหอม</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>กกุคี้</t>
+          <t>น้มอหำ</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>คุบริ้</t>
+          <t>นี้นยาค</t>
         </is>
       </c>
       <c r="E32" t="n">
         <v>6</v>
       </c>
+      <c r="F32" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>75</v>
+        <v>95</v>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>แม็ก</t>
+          <t>กระโดด</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>แมก็</t>
+          <t>ดโกดระ</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>แก๊ม</t>
+          <t>ตระโดก</t>
         </is>
       </c>
       <c r="E33" t="n">
-        <v>4</v>
+        <v>6</v>
+      </c>
+      <c r="F33" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>82</v>
+        <v>10</v>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>แว่นตา</t>
+          <t>ค้างคาว</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>ว่าตนแ</t>
+          <t>คาค้วาง</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>แย้บคา</t>
+          <t>ค้นถาพล</t>
         </is>
       </c>
       <c r="E34" t="n">
+        <v>7</v>
+      </c>
+      <c r="F34" t="n">
         <v>6</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>87</v>
+        <v>22</v>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>นกยูง</t>
+          <t>หนังสือ</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>ยูกนง</t>
+          <t>สัหอืนง</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>นดถูค</t>
+          <t>หกันพีบ</t>
         </is>
       </c>
       <c r="E35" t="n">
+        <v>7</v>
+      </c>
+      <c r="F35" t="n">
         <v>5</v>
       </c>
     </row>
     <row r="36">
-      <c r="A36" t="n">
-        <v>88</v>
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>23a</t>
+        </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>น้ำหอม</t>
+          <t>กระต่าย</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>น้มอหำ</t>
+          <t>รากยต่ะ</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>นี้นยาค</t>
+          <t>ภระค่าบ</t>
         </is>
       </c>
       <c r="E36" t="n">
-        <v>6</v>
+        <v>7</v>
+      </c>
+      <c r="F36" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>89</v>
+        <v>24</v>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>จักรยาน</t>
+          <t>ไม้เท้า</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>นรักายจ</t>
+          <t>ท้เาไม้</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>จัณกทอร</t>
+          <t>ไย้นทีล</t>
         </is>
       </c>
       <c r="E37" t="n">
         <v>7</v>
       </c>
+      <c r="F37" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>93</v>
+        <v>28</v>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>โลมา</t>
+          <t>ของขวัญ</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>มโลา</t>
+          <t>ขัวองญข</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>โบลม</t>
+          <t>ขนาผฟีล</t>
         </is>
       </c>
       <c r="E38" t="n">
-        <v>4</v>
+        <v>7</v>
+      </c>
+      <c r="F38" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>94</v>
+        <v>31</v>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>ยีราฟ</t>
+          <t>เข็มขัด</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>ฟีราย</t>
+          <t>ขเดมัข็</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>ยีหาฝ</t>
+          <t>เน้บลีต</t>
         </is>
       </c>
       <c r="E39" t="n">
+        <v>7</v>
+      </c>
+      <c r="F39" t="n">
         <v>5</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>95</v>
+        <v>61</v>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>แรคคูน</t>
+          <t>รูปปั้น</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>รูคนคแ</t>
+          <t>ป้ปันรู</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>แคกขุย</t>
+          <t>รูฟฝื้อ</t>
         </is>
       </c>
       <c r="E40" t="n">
-        <v>6</v>
+        <v>7</v>
+      </c>
+      <c r="F40" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>กอริลลา</t>
+          <t>จักรยาน</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>อลราลกิ</t>
+          <t>นรักายจ</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>กบคีนรอ</t>
+          <t>จัณกทอร</t>
         </is>
       </c>
       <c r="E41" t="n">
         <v>7</v>
+      </c>
+      <c r="F41" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="42">
@@ -1391,7 +1532,7 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>sub</t>
+          <t>sbu</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
@@ -1402,6 +1543,7 @@
       <c r="E42" t="n">
         <v>3</v>
       </c>
+      <c r="F42" t="inlineStr"/>
     </row>
     <row r="43">
       <c r="A43" t="n">
@@ -1425,6 +1567,7 @@
       <c r="E43" t="n">
         <v>3</v>
       </c>
+      <c r="F43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" t="n">
@@ -1448,6 +1591,7 @@
       <c r="E44" t="n">
         <v>3</v>
       </c>
+      <c r="F44" t="inlineStr"/>
     </row>
     <row r="45">
       <c r="A45" t="n">
@@ -1471,6 +1615,7 @@
       <c r="E45" t="n">
         <v>3</v>
       </c>
+      <c r="F45" t="inlineStr"/>
     </row>
     <row r="46">
       <c r="A46" t="n">
@@ -1488,12 +1633,13 @@
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>sus</t>
+          <t>suw</t>
         </is>
       </c>
       <c r="E46" t="n">
         <v>3</v>
       </c>
+      <c r="F46" t="inlineStr"/>
     </row>
     <row r="47">
       <c r="A47" t="n">
@@ -1517,6 +1663,7 @@
       <c r="E47" t="n">
         <v>3</v>
       </c>
+      <c r="F47" t="inlineStr"/>
     </row>
     <row r="48">
       <c r="A48" t="n">
@@ -1540,6 +1687,7 @@
       <c r="E48" t="n">
         <v>3</v>
       </c>
+      <c r="F48" t="inlineStr"/>
     </row>
     <row r="49">
       <c r="A49" t="n">
@@ -1563,6 +1711,7 @@
       <c r="E49" t="n">
         <v>3</v>
       </c>
+      <c r="F49" t="inlineStr"/>
     </row>
     <row r="50">
       <c r="A50" t="n">
@@ -1586,6 +1735,7 @@
       <c r="E50" t="n">
         <v>4</v>
       </c>
+      <c r="F50" t="inlineStr"/>
     </row>
     <row r="51">
       <c r="A51" t="n">
@@ -1609,6 +1759,7 @@
       <c r="E51" t="n">
         <v>4</v>
       </c>
+      <c r="F51" t="inlineStr"/>
     </row>
     <row r="52">
       <c r="A52" t="n">
@@ -1632,6 +1783,7 @@
       <c r="E52" t="n">
         <v>4</v>
       </c>
+      <c r="F52" t="inlineStr"/>
     </row>
     <row r="53">
       <c r="A53" t="n">
@@ -1649,12 +1801,13 @@
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>vore</t>
+          <t>vrue</t>
         </is>
       </c>
       <c r="E53" t="n">
         <v>4</v>
       </c>
+      <c r="F53" t="inlineStr"/>
     </row>
     <row r="54">
       <c r="A54" t="n">
@@ -1672,12 +1825,13 @@
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>coot</t>
+          <t>comd</t>
         </is>
       </c>
       <c r="E54" t="n">
         <v>4</v>
       </c>
+      <c r="F54" t="inlineStr"/>
     </row>
     <row r="55">
       <c r="A55" t="n">
@@ -1701,6 +1855,7 @@
       <c r="E55" t="n">
         <v>4</v>
       </c>
+      <c r="F55" t="inlineStr"/>
     </row>
     <row r="56">
       <c r="A56" t="n">
@@ -1724,6 +1879,7 @@
       <c r="E56" t="n">
         <v>4</v>
       </c>
+      <c r="F56" t="inlineStr"/>
     </row>
     <row r="57">
       <c r="A57" t="n">
@@ -1747,6 +1903,7 @@
       <c r="E57" t="n">
         <v>4</v>
       </c>
+      <c r="F57" t="inlineStr"/>
     </row>
     <row r="58">
       <c r="A58" t="n">
@@ -1770,6 +1927,7 @@
       <c r="E58" t="n">
         <v>5</v>
       </c>
+      <c r="F58" t="inlineStr"/>
     </row>
     <row r="59">
       <c r="A59" t="n">
@@ -1793,6 +1951,7 @@
       <c r="E59" t="n">
         <v>5</v>
       </c>
+      <c r="F59" t="inlineStr"/>
     </row>
     <row r="60">
       <c r="A60" t="n">
@@ -1816,6 +1975,7 @@
       <c r="E60" t="n">
         <v>5</v>
       </c>
+      <c r="F60" t="inlineStr"/>
     </row>
     <row r="61">
       <c r="A61" t="n">
@@ -1839,6 +1999,7 @@
       <c r="E61" t="n">
         <v>5</v>
       </c>
+      <c r="F61" t="inlineStr"/>
     </row>
     <row r="62">
       <c r="A62" t="n">
@@ -1862,6 +2023,7 @@
       <c r="E62" t="n">
         <v>5</v>
       </c>
+      <c r="F62" t="inlineStr"/>
     </row>
     <row r="63">
       <c r="A63" t="n">
@@ -1885,6 +2047,7 @@
       <c r="E63" t="n">
         <v>5</v>
       </c>
+      <c r="F63" t="inlineStr"/>
     </row>
     <row r="64">
       <c r="A64" t="n">
@@ -1908,6 +2071,7 @@
       <c r="E64" t="n">
         <v>5</v>
       </c>
+      <c r="F64" t="inlineStr"/>
     </row>
     <row r="65">
       <c r="A65" t="n">
@@ -1931,6 +2095,7 @@
       <c r="E65" t="n">
         <v>5</v>
       </c>
+      <c r="F65" t="inlineStr"/>
     </row>
     <row r="66">
       <c r="A66" t="n">
@@ -1954,6 +2119,7 @@
       <c r="E66" t="n">
         <v>6</v>
       </c>
+      <c r="F66" t="inlineStr"/>
     </row>
     <row r="67">
       <c r="A67" t="n">
@@ -1977,6 +2143,7 @@
       <c r="E67" t="n">
         <v>6</v>
       </c>
+      <c r="F67" t="inlineStr"/>
     </row>
     <row r="68">
       <c r="A68" t="n">
@@ -2000,6 +2167,7 @@
       <c r="E68" t="n">
         <v>6</v>
       </c>
+      <c r="F68" t="inlineStr"/>
     </row>
     <row r="69">
       <c r="A69" t="n">
@@ -2023,6 +2191,7 @@
       <c r="E69" t="n">
         <v>6</v>
       </c>
+      <c r="F69" t="inlineStr"/>
     </row>
     <row r="70">
       <c r="A70" t="n">
@@ -2046,6 +2215,7 @@
       <c r="E70" t="n">
         <v>6</v>
       </c>
+      <c r="F70" t="inlineStr"/>
     </row>
     <row r="71">
       <c r="A71" t="n">
@@ -2069,6 +2239,7 @@
       <c r="E71" t="n">
         <v>6</v>
       </c>
+      <c r="F71" t="inlineStr"/>
     </row>
     <row r="72">
       <c r="A72" t="n">
@@ -2092,6 +2263,7 @@
       <c r="E72" t="n">
         <v>6</v>
       </c>
+      <c r="F72" t="inlineStr"/>
     </row>
     <row r="73">
       <c r="A73" t="n">
@@ -2115,6 +2287,7 @@
       <c r="E73" t="n">
         <v>6</v>
       </c>
+      <c r="F73" t="inlineStr"/>
     </row>
     <row r="74">
       <c r="A74" t="n">
@@ -2138,6 +2311,7 @@
       <c r="E74" t="n">
         <v>7</v>
       </c>
+      <c r="F74" t="inlineStr"/>
     </row>
     <row r="75">
       <c r="A75" t="n">
@@ -2161,6 +2335,7 @@
       <c r="E75" t="n">
         <v>7</v>
       </c>
+      <c r="F75" t="inlineStr"/>
     </row>
     <row r="76">
       <c r="A76" t="n">
@@ -2184,6 +2359,7 @@
       <c r="E76" t="n">
         <v>7</v>
       </c>
+      <c r="F76" t="inlineStr"/>
     </row>
     <row r="77">
       <c r="A77" t="n">
@@ -2207,6 +2383,7 @@
       <c r="E77" t="n">
         <v>7</v>
       </c>
+      <c r="F77" t="inlineStr"/>
     </row>
     <row r="78">
       <c r="A78" t="n">
@@ -2230,6 +2407,7 @@
       <c r="E78" t="n">
         <v>7</v>
       </c>
+      <c r="F78" t="inlineStr"/>
     </row>
     <row r="79">
       <c r="A79" t="n">
@@ -2253,6 +2431,7 @@
       <c r="E79" t="n">
         <v>7</v>
       </c>
+      <c r="F79" t="inlineStr"/>
     </row>
     <row r="80">
       <c r="A80" t="n">
@@ -2276,6 +2455,7 @@
       <c r="E80" t="n">
         <v>7</v>
       </c>
+      <c r="F80" t="inlineStr"/>
     </row>
     <row r="81">
       <c r="A81" t="n">
@@ -2299,6 +2479,7 @@
       <c r="E81" t="n">
         <v>7</v>
       </c>
+      <c r="F81" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>